<commit_message>
Adding support for debugging
</commit_message>
<xml_diff>
--- a/analysis/data_provider_example.xlsx
+++ b/analysis/data_provider_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blakeblackwell/Dev/Github/personal/SBTi/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE8871F-54B9-074A-BBFE-65AB4CB3EAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC1F44A-60FF-8846-9CC4-73BEAE1081D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>company_name</t>
   </si>
@@ -196,6 +196,39 @@
   </si>
   <si>
     <t>engagement_target</t>
+  </si>
+  <si>
+    <t>s1s2_wats</t>
+  </si>
+  <si>
+    <t>s3_wats</t>
+  </si>
+  <si>
+    <t>s1s2s3_wats</t>
+  </si>
+  <si>
+    <t>s1s2_tets</t>
+  </si>
+  <si>
+    <t>Portfolio Temperature Score</t>
+  </si>
+  <si>
+    <t>s3_tets</t>
+  </si>
+  <si>
+    <t>s1s2s3_tets</t>
+  </si>
+  <si>
+    <t>s1s2_rots</t>
+  </si>
+  <si>
+    <t>owned_emissions_s1s2_rots</t>
+  </si>
+  <si>
+    <t>owned_emissions_s3</t>
+  </si>
+  <si>
+    <t>s3_rots</t>
   </si>
 </sst>
 </file>
@@ -231,7 +264,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +295,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -275,12 +314,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -297,25 +335,13 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -334,20 +360,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -375,7 +387,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K11" totalsRowShown="0" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K11" totalsRowShown="0" tableBorderDxfId="4">
   <autoFilter ref="A1:K11" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
@@ -386,7 +398,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="company_revenue"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="company_market_cap"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="company_enterprise_value"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="company_total_assets" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="company_total_assets" dataDxfId="3"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="company_cash_equivalents"/>
     <tableColumn id="4" xr3:uid="{858E90EA-527D-1A41-96F3-70373674DFD3}" name="sbti_validated"/>
   </tableColumns>
@@ -395,8 +407,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:O111" totalsRowShown="0">
-  <autoFilter ref="A1:O111" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:O11" totalsRowShown="0">
+  <autoFilter ref="A1:O11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="company_id"/>
@@ -684,7 +696,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -698,6 +710,7 @@
     <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -749,7 +762,7 @@
         <v>20000</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -781,7 +794,7 @@
         <v>2500</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>76000</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -813,7 +826,7 @@
         <v>750000</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>750000</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -845,7 +858,7 @@
         <v>3000000</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -877,7 +890,7 @@
         <v>50000</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>3000000</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -909,7 +922,7 @@
         <v>500000</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -941,7 +954,7 @@
         <v>500</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -973,7 +986,7 @@
         <v>35000</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>2500000</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1005,7 +1018,7 @@
         <v>4000000</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>8000000</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1037,7 +1050,7 @@
         <v>2000</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>250000</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1066,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O122"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1570,10 +1583,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="6:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1587,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2106B7-AABC-6248-8796-3171DA24AD96}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1601,22 +1610,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1630,11 +1639,11 @@
       <c r="C2">
         <v>10001</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>0.1</v>
       </c>
       <c r="E2">
-        <v>35000000</v>
+        <v>25000</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1650,11 +1659,11 @@
       <c r="C3">
         <v>10002</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>0.1</v>
       </c>
       <c r="E3">
-        <v>10000000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1667,11 +1676,11 @@
       <c r="C4">
         <v>10003</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.1</v>
       </c>
       <c r="E4">
-        <v>10000000</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1684,11 +1693,11 @@
       <c r="C5">
         <v>10004</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.1</v>
       </c>
       <c r="E5">
-        <v>10000000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1701,11 +1710,11 @@
       <c r="C6">
         <v>10005</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>0.1</v>
       </c>
       <c r="E6">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1718,11 +1727,11 @@
       <c r="C7">
         <v>10006</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>0.1</v>
       </c>
       <c r="E7">
-        <v>10000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1735,11 +1744,11 @@
       <c r="C8">
         <v>10007</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <v>0.1</v>
       </c>
       <c r="E8">
-        <v>10000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1752,11 +1761,11 @@
       <c r="C9">
         <v>10008</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>0.1</v>
       </c>
       <c r="E9">
-        <v>10000000</v>
+        <v>400000</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1769,11 +1778,11 @@
       <c r="C10">
         <v>10009</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <v>0.1</v>
       </c>
       <c r="E10">
-        <v>10000000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1786,11 +1795,11 @@
       <c r="C11">
         <v>10010</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>0.1</v>
       </c>
       <c r="E11">
-        <v>10000000</v>
+        <v>150000</v>
       </c>
     </row>
   </sheetData>
@@ -1800,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22944271-7D1A-D94D-94D4-7E7FB938DDE4}">
-  <dimension ref="A1:AB11"/>
+  <dimension ref="A1:AN12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1817,1233 +1826,1791 @@
     <col min="11" max="11" width="14.1640625" customWidth="1"/>
     <col min="12" max="12" width="23.1640625" customWidth="1"/>
     <col min="13" max="13" width="18.1640625" customWidth="1"/>
-    <col min="14" max="15" width="24.83203125" customWidth="1"/>
-    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.33203125" customWidth="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="24.83203125" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" customWidth="1"/>
+    <col min="20" max="22" width="19.33203125" customWidth="1"/>
+    <col min="23" max="26" width="10.83203125" customWidth="1"/>
+    <col min="29" max="29" width="21" customWidth="1"/>
+    <col min="30" max="30" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AA1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AC1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="str">
+      <c r="AE1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL1" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="str">
         <f>fundamental_data!A2</f>
         <v>Company A</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <f>fundamental_data!B2</f>
         <v>10001</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <f>fundamental_data!C2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="str">
+      <c r="D2" s="3" t="str">
         <f>target_data!C2</f>
         <v>Absolute</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <f>target_data!D2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <f>fundamental_data!D2</f>
         <v>10000</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <f>fundamental_data!E2</f>
         <v>20000</v>
       </c>
-      <c r="H2" s="4" t="str">
+      <c r="H2" s="3" t="str">
         <f>target_data!E2</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <f>target_data!F2</f>
         <v>0.8</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <f>target_data!G2</f>
         <v>1</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <f>target_data!H2</f>
         <v>0.5</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <f>target_data!J2</f>
         <v>2020</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <f>target_data!K2</f>
         <v>2034</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="3">
         <f>target_data!I2</f>
         <v>0.7</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="15">
+        <f>portfolio!E2</f>
+        <v>25000</v>
+      </c>
+      <c r="P2" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>50000</v>
+      </c>
+      <c r="Q2" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P2" s="8">
+      <c r="R2" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="S2" s="5">
         <f ca="1">YEAR(TODAY())</f>
         <v>2021</v>
       </c>
-      <c r="R2" s="6">
-        <f t="shared" ref="R2:R11" ca="1" si="0">M2-Q2</f>
+      <c r="T2" s="5">
+        <f t="shared" ref="T2:T11" ca="1" si="0">M2-S2</f>
         <v>13</v>
       </c>
-      <c r="S2" s="6">
-        <f t="shared" ref="S2:S11" si="1">M2-L2</f>
+      <c r="U2" s="5">
+        <f t="shared" ref="U2:U11" si="1">M2-L2</f>
         <v>14</v>
       </c>
-      <c r="T2" s="6" t="str">
-        <f ca="1">IF(R2&lt;4,"short",IF(R2&lt;15,"mid","long"))</f>
+      <c r="V2" s="5" t="str">
+        <f ca="1">IF(T2&lt;4,"short",IF(T2&lt;15,"mid","long"))</f>
         <v>mid</v>
       </c>
-      <c r="U2" s="6">
-        <f t="shared" ref="U2:U11" si="2">IF(I2&lt;0.95,I2*N2,N2)</f>
+      <c r="W2" s="5">
+        <f t="shared" ref="W2:W11" si="2">IF(I2&lt;0.95,I2*N2,N2)</f>
         <v>0.55999999999999994</v>
       </c>
-      <c r="V2" s="6">
-        <f t="shared" ref="V2:V11" si="3">IF(K2&lt;0.67,K2*N2,N2)</f>
+      <c r="X2" s="5">
+        <f t="shared" ref="X2:X11" si="3">IF(K2&lt;0.67,K2*N2,N2)</f>
         <v>0.35</v>
       </c>
-      <c r="W2" s="6">
-        <f t="shared" ref="W2:W11" si="4">U2/S2</f>
+      <c r="Y2" s="5">
+        <f t="shared" ref="Y2:Y11" si="4">W2/U2</f>
         <v>3.9999999999999994E-2</v>
       </c>
-      <c r="X2" s="6">
-        <f t="shared" ref="X2:X11" si="5">V2/S2</f>
+      <c r="Z2" s="5">
+        <f t="shared" ref="Z2:Z11" si="5">X2/U2</f>
         <v>2.4999999999999998E-2</v>
       </c>
-      <c r="Y2" s="10">
-        <f t="shared" ref="Y2:Y11" si="6">(W2*O2*100)+P2</f>
-        <v>1.4479450000000003</v>
-      </c>
-      <c r="Z2" s="10">
-        <f t="shared" ref="Z2:Z11" si="7">(X2*O2*100)+P2</f>
-        <v>1.9164385000000002</v>
-      </c>
-      <c r="AA2" s="10">
-        <f t="shared" ref="AA2:AA11" si="8">G2/SUM(F2:G2)</f>
+      <c r="AA2" s="9">
+        <f>ROUND((Y2*Q2*100)+R2,2)</f>
+        <v>1.45</v>
+      </c>
+      <c r="AB2" s="9">
+        <f>ROUND((Z2*Q2*100)+R2,2)</f>
+        <v>1.92</v>
+      </c>
+      <c r="AC2" s="9">
+        <f t="shared" ref="AC2:AC11" si="6">G2/SUM(F2:G2)</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="AB2" s="10">
-        <f t="shared" ref="AB2:AB11" si="9">IF(AA2&lt;0.4,Y2,((Y2*F2)+(Z2*G2))/SUM(F2:G2))</f>
-        <v>1.7602740000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="str">
+      <c r="AD2" s="9">
+        <f>ROUND(IF(AC2&lt;0.4,AA2,((AA2*F2)+(AB2*G2))/SUM(F2:G2)),2)</f>
+        <v>1.76</v>
+      </c>
+      <c r="AE2" s="15">
+        <f>($O$2*AA2)/SUM($O$2:$O$11)</f>
+        <v>4.9657534246575347E-3</v>
+      </c>
+      <c r="AF2" s="15">
+        <f>($O2*AB2)/SUM($O$2:$O$11)</f>
+        <v>6.5753424657534251E-3</v>
+      </c>
+      <c r="AG2" s="15">
+        <f>($O2*AD2)/SUM($O$2:$O$11)</f>
+        <v>6.0273972602739728E-3</v>
+      </c>
+      <c r="AH2" s="15">
+        <f>$F2/SUM($F$2:$F$11)*$AA2</f>
+        <v>8.7113247221387807E-4</v>
+      </c>
+      <c r="AI2" s="15">
+        <f>G2/SUM(G$2:G$11)*$AB2</f>
+        <v>4.5933014354066978E-3</v>
+      </c>
+      <c r="AJ2" s="15">
+        <f>SUM(F2:G2)/SUM(F$2:G$11)*AD2</f>
+        <v>2.1115776844631072E-3</v>
+      </c>
+      <c r="AK2" s="15">
+        <f>($O2/$P2)*F2</f>
+        <v>5000</v>
+      </c>
+      <c r="AL2" s="15">
+        <f>(AK2/SUM(AK$2:AK$11))*AA2</f>
+        <v>1.0144084041373627E-3</v>
+      </c>
+      <c r="AM2" s="15">
+        <f>($O2/$P2)*G2</f>
+        <v>10000</v>
+      </c>
+      <c r="AN2" s="15">
+        <f>(AM2/SUM(AM$2:AM$11))*AB2</f>
+        <v>4.5572020678137821E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="str">
         <f>fundamental_data!A3</f>
         <v>Company B</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <f>fundamental_data!B3</f>
         <v>10002</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <f>fundamental_data!C3</f>
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="str">
+      <c r="D3" s="3" t="str">
         <f>target_data!C3</f>
         <v>Absolute</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <f>target_data!D3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <f>fundamental_data!D3</f>
         <v>5000</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <f>fundamental_data!E3</f>
         <v>2500</v>
       </c>
-      <c r="H3" s="4" t="str">
+      <c r="H3" s="3" t="str">
         <f>target_data!E3</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <f>target_data!F3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <f>target_data!G3</f>
         <v>1</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <f>target_data!H3</f>
         <v>1</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <f>target_data!J3</f>
         <v>2020</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <f>target_data!K3</f>
         <v>2034</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="3">
         <f>target_data!I3</f>
         <v>0.7</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="15">
+        <f>portfolio!E3</f>
+        <v>50000</v>
+      </c>
+      <c r="P3" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>76000</v>
+      </c>
+      <c r="Q3" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P3" s="8">
+      <c r="R3" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q3" s="6">
-        <f t="shared" ref="Q3:Q11" ca="1" si="10">YEAR(TODAY())</f>
+      <c r="S3" s="5">
+        <f t="shared" ref="S3:S11" ca="1" si="7">YEAR(TODAY())</f>
         <v>2021</v>
       </c>
-      <c r="R3" s="6">
+      <c r="T3" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S3" s="6">
+      <c r="U3" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T3" s="6" t="str">
-        <f t="shared" ref="T3:T11" ca="1" si="11">IF(R3&lt;4,"short",IF(R3&lt;15,"mid","long"))</f>
+      <c r="V3" s="5" t="str">
+        <f t="shared" ref="V3:V11" ca="1" si="8">IF(T3&lt;4,"short",IF(T3&lt;15,"mid","long"))</f>
         <v>mid</v>
       </c>
-      <c r="U3" s="6">
+      <c r="W3" s="5">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="V3" s="6">
+      <c r="X3" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W3" s="6">
+      <c r="Y3" s="5">
         <f t="shared" si="4"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="X3" s="6">
+      <c r="Z3" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y3" s="10">
+      <c r="AA3" s="9">
+        <f t="shared" ref="AA3:AA11" si="9">ROUND((Y3*Q3*100)+R3,2)</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB3" s="9">
+        <f t="shared" ref="AB3:AB11" si="10">ROUND((Z3*Q3*100)+R3,2)</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC3" s="9">
         <f t="shared" si="6"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="Z3" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA3" s="10">
-        <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AB3" s="10">
-        <f t="shared" si="9"/>
-        <v>1.1356160000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="str">
+      <c r="AD3" s="9">
+        <f t="shared" ref="AD3:AD11" si="11">ROUND(IF(AC3&lt;0.4,AA3,((AA3*F3)+(AB3*G3))/SUM(F3:G3)),2)</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AE3" s="15">
+        <f>(O3*AA3)/SUM($O$2:$O$11)</f>
+        <v>7.8082191780821904E-3</v>
+      </c>
+      <c r="AF3" s="15">
+        <f>($O3*AB3)/SUM($O$2:$O$11)</f>
+        <v>7.8082191780821904E-3</v>
+      </c>
+      <c r="AG3" s="15">
+        <f>($O3*AD3)/SUM($O$2:$O$11)</f>
+        <v>7.8082191780821904E-3</v>
+      </c>
+      <c r="AH3" s="15">
+        <f t="shared" ref="AH3:AH11" si="12">$F3/SUM($F$2:$F$11)*$AA3</f>
+        <v>3.4244517873235203E-4</v>
+      </c>
+      <c r="AI3" s="15">
+        <f>G3/SUM(G$2:G$11)*$AB3</f>
+        <v>3.4090909090909088E-4</v>
+      </c>
+      <c r="AJ3" s="15">
+        <f>SUM(F3:G3)/SUM(F$2:G$11)*AD3</f>
+        <v>3.4193161367726451E-4</v>
+      </c>
+      <c r="AK3" s="15">
+        <f t="shared" ref="AK3:AK11" si="13">($O3/$P3)*F3</f>
+        <v>3289.4736842105267</v>
+      </c>
+      <c r="AL3" s="15">
+        <f t="shared" ref="AL3:AL11" si="14">(AK3/SUM(AK$2:AK$11))*AA3</f>
+        <v>5.2469400214001519E-4</v>
+      </c>
+      <c r="AM3" s="15">
+        <f t="shared" ref="AM3:AM11" si="15">($O3/$P3)*G3</f>
+        <v>1644.7368421052633</v>
+      </c>
+      <c r="AN3" s="15">
+        <f t="shared" ref="AN3:AN11" si="16">AM3/SUM(AM$2:AM$11)*AB3</f>
+        <v>4.4503926443493976E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="str">
         <f>fundamental_data!A4</f>
         <v>Company C</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <f>fundamental_data!B4</f>
         <v>10003</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f>fundamental_data!C4</f>
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="str">
+      <c r="D4" s="3" t="str">
         <f>target_data!C4</f>
         <v>Absolute</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <f>target_data!D4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <f>fundamental_data!D4</f>
         <v>1000000</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <f>fundamental_data!E4</f>
         <v>750000</v>
       </c>
-      <c r="H4" s="4" t="str">
+      <c r="H4" s="3" t="str">
         <f>target_data!E4</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <f>target_data!F4</f>
         <v>1</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <f>target_data!G4</f>
         <v>1</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <f>target_data!H4</f>
         <v>0.65</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <f>target_data!J4</f>
         <v>2020</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <f>target_data!K4</f>
         <v>2034</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <f>target_data!I4</f>
         <v>0.7</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="15">
+        <f>portfolio!E4</f>
+        <v>75000</v>
+      </c>
+      <c r="P4" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>750000</v>
+      </c>
+      <c r="Q4" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P4" s="8">
+      <c r="R4" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q4" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S4" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R4" s="6">
+      <c r="T4" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S4" s="6">
+      <c r="U4" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T4" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V4" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U4" s="6">
+      <c r="W4" s="5">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="V4" s="6">
+      <c r="X4" s="5">
         <f t="shared" si="3"/>
         <v>0.45499999999999996</v>
       </c>
-      <c r="W4" s="6">
+      <c r="Y4" s="5">
         <f t="shared" si="4"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="X4" s="6">
+      <c r="Z4" s="5">
         <f t="shared" si="5"/>
         <v>3.2499999999999994E-2</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="AA4" s="9">
+        <f t="shared" si="9"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB4" s="9">
+        <f t="shared" si="10"/>
+        <v>1.68</v>
+      </c>
+      <c r="AC4" s="9">
         <f t="shared" si="6"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="Z4" s="10">
-        <f t="shared" si="7"/>
-        <v>1.6821917500000003</v>
-      </c>
-      <c r="AA4" s="10">
-        <f t="shared" si="8"/>
         <v>0.42857142857142855</v>
       </c>
-      <c r="AB4" s="10">
-        <f t="shared" si="9"/>
-        <v>1.3698627500000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="str">
+      <c r="AD4" s="9">
+        <f t="shared" si="11"/>
+        <v>1.37</v>
+      </c>
+      <c r="AE4" s="15">
+        <f>(O4*AA4)/SUM($O$2:$O$11)</f>
+        <v>1.1712328767123286E-2</v>
+      </c>
+      <c r="AF4" s="15">
+        <f>($O4*AB4)/SUM($O$2:$O$11)</f>
+        <v>1.7260273972602741E-2</v>
+      </c>
+      <c r="AG4" s="15">
+        <f>($O4*AD4)/SUM($O$2:$O$11)</f>
+        <v>1.4075342465753427E-2</v>
+      </c>
+      <c r="AH4" s="15">
+        <f t="shared" si="12"/>
+        <v>6.8489035746470403E-2</v>
+      </c>
+      <c r="AI4" s="15">
+        <f>G4/SUM(G$2:G$11)*$AB4</f>
+        <v>0.15071770334928228</v>
+      </c>
+      <c r="AJ4" s="15">
+        <f>SUM(F4:G4)/SUM(F$2:G$11)*AD4</f>
+        <v>9.588082383523297E-2</v>
+      </c>
+      <c r="AK4" s="15">
+        <f t="shared" si="13"/>
+        <v>100000</v>
+      </c>
+      <c r="AL4" s="15">
+        <f t="shared" si="14"/>
+        <v>1.5950697665056458E-2</v>
+      </c>
+      <c r="AM4" s="15">
+        <f t="shared" si="15"/>
+        <v>75000</v>
+      </c>
+      <c r="AN4" s="15">
+        <f t="shared" si="16"/>
+        <v>2.9906638570027944E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="str">
         <f>fundamental_data!A5</f>
         <v>Company D</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <f>fundamental_data!B5</f>
         <v>10004</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="11">
         <f>fundamental_data!C5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="str">
+      <c r="D5" s="3" t="str">
         <f>target_data!C5</f>
         <v>Absolute</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <f>target_data!D5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <f>fundamental_data!D5</f>
         <v>5000000</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <f>fundamental_data!E5</f>
         <v>3000000</v>
       </c>
-      <c r="H5" s="4" t="str">
+      <c r="H5" s="3" t="str">
         <f>target_data!E5</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <f>target_data!F5</f>
         <v>0.65</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <f>target_data!G5</f>
         <v>1</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <f>target_data!H5</f>
         <v>0.96</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <f>target_data!J5</f>
         <v>2020</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <f>target_data!K5</f>
         <v>2034</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <f>target_data!I5</f>
         <v>0.7</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="15">
+        <f>portfolio!E5</f>
+        <v>100000</v>
+      </c>
+      <c r="P5" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>80000</v>
+      </c>
+      <c r="Q5" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P5" s="8">
+      <c r="R5" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q5" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S5" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R5" s="6">
+      <c r="T5" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S5" s="6">
+      <c r="U5" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T5" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V5" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U5" s="6">
+      <c r="W5" s="5">
         <f t="shared" si="2"/>
         <v>0.45499999999999996</v>
       </c>
-      <c r="V5" s="6">
+      <c r="X5" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W5" s="6">
+      <c r="Y5" s="5">
         <f t="shared" si="4"/>
         <v>3.2499999999999994E-2</v>
       </c>
-      <c r="X5" s="6">
+      <c r="Z5" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="AA5" s="9">
+        <f t="shared" si="9"/>
+        <v>1.68</v>
+      </c>
+      <c r="AB5" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC5" s="9">
         <f t="shared" si="6"/>
-        <v>1.6821917500000003</v>
-      </c>
-      <c r="Z5" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA5" s="10">
-        <f t="shared" si="8"/>
         <v>0.375</v>
       </c>
-      <c r="AB5" s="10">
-        <f t="shared" si="9"/>
-        <v>1.6821917500000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="str">
+      <c r="AD5" s="9">
+        <f t="shared" si="11"/>
+        <v>1.68</v>
+      </c>
+      <c r="AE5" s="15">
+        <f>(O5*AA5)/SUM($O$2:$O$11)</f>
+        <v>2.3013698630136987E-2</v>
+      </c>
+      <c r="AF5" s="15">
+        <f>($O5*AB5)/SUM($O$2:$O$11)</f>
+        <v>1.5616438356164381E-2</v>
+      </c>
+      <c r="AG5" s="15">
+        <f>($O5*AD5)/SUM($O$2:$O$11)</f>
+        <v>2.3013698630136987E-2</v>
+      </c>
+      <c r="AH5" s="15">
+        <f t="shared" si="12"/>
+        <v>0.50465605286872939</v>
+      </c>
+      <c r="AI5" s="15">
+        <f>G5/SUM(G$2:G$11)*$AB5</f>
+        <v>0.40909090909090906</v>
+      </c>
+      <c r="AJ5" s="15">
+        <f>SUM(F5:G5)/SUM(F$2:G$11)*AD5</f>
+        <v>0.53749250149969996</v>
+      </c>
+      <c r="AK5" s="15">
+        <f t="shared" si="13"/>
+        <v>6250000</v>
+      </c>
+      <c r="AL5" s="15">
+        <f t="shared" si="14"/>
+        <v>1.4691432059920424</v>
+      </c>
+      <c r="AM5" s="15">
+        <f t="shared" si="15"/>
+        <v>3750000</v>
+      </c>
+      <c r="AN5" s="15">
+        <f t="shared" si="16"/>
+        <v>1.0146895229116624</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="str">
         <f>fundamental_data!A6</f>
         <v>Company E</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <f>fundamental_data!B6</f>
         <v>10005</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f>fundamental_data!C6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="4" t="str">
+      <c r="D6" s="3" t="str">
         <f>target_data!C6</f>
         <v>Absolute</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <f>target_data!D6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <f>fundamental_data!D6</f>
         <v>250000</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f>fundamental_data!E6</f>
         <v>50000</v>
       </c>
-      <c r="H6" s="4" t="str">
+      <c r="H6" s="3" t="str">
         <f>target_data!E6</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <f>target_data!F6</f>
         <v>0.66</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <f>target_data!G6</f>
         <v>1</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <f>target_data!H6</f>
         <v>0.94</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <f>target_data!J6</f>
         <v>2020</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <f>target_data!K6</f>
         <v>2034</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <f>target_data!I6</f>
         <v>0.7</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="15">
+        <f>portfolio!E6</f>
+        <v>1000000</v>
+      </c>
+      <c r="P6" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>3000000</v>
+      </c>
+      <c r="Q6" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P6" s="8">
+      <c r="R6" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q6" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S6" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R6" s="6">
+      <c r="T6" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S6" s="6">
+      <c r="U6" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T6" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V6" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U6" s="6">
+      <c r="W6" s="5">
         <f t="shared" si="2"/>
         <v>0.46199999999999997</v>
       </c>
-      <c r="V6" s="6">
+      <c r="X6" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W6" s="6">
+      <c r="Y6" s="5">
         <f t="shared" si="4"/>
         <v>3.2999999999999995E-2</v>
       </c>
-      <c r="X6" s="6">
+      <c r="Z6" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="AA6" s="9">
+        <f t="shared" si="9"/>
+        <v>1.67</v>
+      </c>
+      <c r="AB6" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC6" s="9">
         <f t="shared" si="6"/>
-        <v>1.6665753000000003</v>
-      </c>
-      <c r="Z6" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA6" s="10">
-        <f t="shared" si="8"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="AB6" s="10">
-        <f t="shared" si="9"/>
-        <v>1.6665753000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="str">
+      <c r="AD6" s="9">
+        <f t="shared" si="11"/>
+        <v>1.67</v>
+      </c>
+      <c r="AE6" s="15">
+        <f>(O6*AA6)/SUM($O$2:$O$11)</f>
+        <v>0.22876712328767124</v>
+      </c>
+      <c r="AF6" s="15">
+        <f>($O6*AB6)/SUM($O$2:$O$11)</f>
+        <v>0.15616438356164383</v>
+      </c>
+      <c r="AG6" s="15">
+        <f>($O6*AD6)/SUM($O$2:$O$11)</f>
+        <v>0.22876712328767124</v>
+      </c>
+      <c r="AH6" s="15">
+        <f t="shared" si="12"/>
+        <v>2.5082607389606489E-2</v>
+      </c>
+      <c r="AI6" s="15">
+        <f>G6/SUM(G$2:G$11)*$AB6</f>
+        <v>6.8181818181818179E-3</v>
+      </c>
+      <c r="AJ6" s="15">
+        <f>SUM(F6:G6)/SUM(F$2:G$11)*AD6</f>
+        <v>2.0035992801439712E-2</v>
+      </c>
+      <c r="AK6" s="15">
+        <f t="shared" si="13"/>
+        <v>83333.333333333328</v>
+      </c>
+      <c r="AL6" s="15">
+        <f t="shared" si="14"/>
+        <v>1.9471977412751671E-2</v>
+      </c>
+      <c r="AM6" s="15">
+        <f t="shared" si="15"/>
+        <v>16666.666666666664</v>
+      </c>
+      <c r="AN6" s="15">
+        <f t="shared" si="16"/>
+        <v>4.5097312129407218E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="str">
         <f>fundamental_data!A7</f>
         <v>Company F</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <f>fundamental_data!B7</f>
         <v>10006</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <f>fundamental_data!C7</f>
         <v>0</v>
       </c>
-      <c r="D7" s="4" t="str">
+      <c r="D7" s="3" t="str">
         <f>target_data!C7</f>
         <v>Absolute</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f>target_data!D7</f>
         <v>0</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <f>fundamental_data!D7</f>
         <v>300000</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <f>fundamental_data!E7</f>
         <v>500000</v>
       </c>
-      <c r="H7" s="4" t="str">
+      <c r="H7" s="3" t="str">
         <f>target_data!E7</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <f>target_data!F7</f>
         <v>1</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <f>target_data!G7</f>
         <v>1</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <f>target_data!H7</f>
         <v>1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <f>target_data!J7</f>
         <v>2020</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <f>target_data!K7</f>
         <v>2034</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <f>target_data!I7</f>
         <v>0.7</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="15">
+        <f>portfolio!E7</f>
+        <v>2000000</v>
+      </c>
+      <c r="P7" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>10000000</v>
+      </c>
+      <c r="Q7" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P7" s="8">
+      <c r="R7" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q7" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S7" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R7" s="6">
+      <c r="T7" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S7" s="6">
+      <c r="U7" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T7" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V7" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U7" s="6">
+      <c r="W7" s="5">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="V7" s="6">
+      <c r="X7" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W7" s="6">
+      <c r="Y7" s="5">
         <f t="shared" si="4"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="X7" s="6">
+      <c r="Z7" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="AA7" s="9">
+        <f t="shared" si="9"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB7" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC7" s="9">
         <f t="shared" si="6"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="Z7" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA7" s="10">
-        <f t="shared" si="8"/>
         <v>0.625</v>
       </c>
-      <c r="AB7" s="10">
-        <f t="shared" si="9"/>
-        <v>1.1356160000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="str">
+      <c r="AD7" s="9">
+        <f t="shared" si="11"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AE7" s="15">
+        <f>(O7*AA7)/SUM($O$2:$O$11)</f>
+        <v>0.31232876712328766</v>
+      </c>
+      <c r="AF7" s="15">
+        <f>($O7*AB7)/SUM($O$2:$O$11)</f>
+        <v>0.31232876712328766</v>
+      </c>
+      <c r="AG7" s="15">
+        <f>($O7*AD7)/SUM($O$2:$O$11)</f>
+        <v>0.31232876712328766</v>
+      </c>
+      <c r="AH7" s="15">
+        <f t="shared" si="12"/>
+        <v>2.0546710723941122E-2</v>
+      </c>
+      <c r="AI7" s="15">
+        <f>G7/SUM(G$2:G$11)*$AB7</f>
+        <v>6.8181818181818177E-2</v>
+      </c>
+      <c r="AJ7" s="15">
+        <f>SUM(F7:G7)/SUM(F$2:G$11)*AD7</f>
+        <v>3.6472705458908218E-2</v>
+      </c>
+      <c r="AK7" s="15">
+        <f t="shared" si="13"/>
+        <v>60000</v>
+      </c>
+      <c r="AL7" s="15">
+        <f t="shared" si="14"/>
+        <v>9.570418599033877E-3</v>
+      </c>
+      <c r="AM7" s="15">
+        <f t="shared" si="15"/>
+        <v>100000</v>
+      </c>
+      <c r="AN7" s="15">
+        <f t="shared" si="16"/>
+        <v>2.7058387277644331E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="str">
         <f>fundamental_data!A8</f>
         <v>Company G</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <f>fundamental_data!B8</f>
         <v>10007</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <f>fundamental_data!C8</f>
         <v>0</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D8" s="3" t="str">
         <f>target_data!C8</f>
         <v>Absolute</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <f>target_data!D8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <f>fundamental_data!D8</f>
         <v>1000</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f>fundamental_data!E8</f>
         <v>500</v>
       </c>
-      <c r="H8" s="4" t="str">
+      <c r="H8" s="3" t="str">
         <f>target_data!E8</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <f>target_data!F8</f>
         <v>0.5</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <f>target_data!G8</f>
         <v>1</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <f>target_data!H8</f>
         <v>0.9</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <f>target_data!J8</f>
         <v>2020</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <f>target_data!K8</f>
         <v>2034</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <f>target_data!I8</f>
         <v>0.7</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="15">
+        <f>portfolio!E8</f>
+        <v>3000000</v>
+      </c>
+      <c r="P8" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>500000</v>
+      </c>
+      <c r="Q8" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P8" s="8">
+      <c r="R8" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q8" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S8" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R8" s="6">
+      <c r="T8" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S8" s="6">
+      <c r="U8" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T8" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V8" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U8" s="6">
+      <c r="W8" s="5">
         <f t="shared" si="2"/>
         <v>0.35</v>
       </c>
-      <c r="V8" s="6">
+      <c r="X8" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W8" s="6">
+      <c r="Y8" s="5">
         <f t="shared" si="4"/>
         <v>2.4999999999999998E-2</v>
       </c>
-      <c r="X8" s="6">
+      <c r="Z8" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y8" s="10">
+      <c r="AA8" s="9">
+        <f t="shared" si="9"/>
+        <v>1.92</v>
+      </c>
+      <c r="AB8" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC8" s="9">
         <f t="shared" si="6"/>
-        <v>1.9164385000000002</v>
-      </c>
-      <c r="Z8" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA8" s="10">
-        <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AB8" s="10">
-        <f t="shared" si="9"/>
-        <v>1.9164385000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="str">
+      <c r="AD8" s="9">
+        <f t="shared" si="11"/>
+        <v>1.92</v>
+      </c>
+      <c r="AE8" s="15">
+        <f>(O8*AA8)/SUM($O$2:$O$11)</f>
+        <v>0.78904109589041094</v>
+      </c>
+      <c r="AF8" s="15">
+        <f>($O8*AB8)/SUM($O$2:$O$11)</f>
+        <v>0.46849315068493147</v>
+      </c>
+      <c r="AG8" s="15">
+        <f>($O8*AD8)/SUM($O$2:$O$11)</f>
+        <v>0.78904109589041094</v>
+      </c>
+      <c r="AH8" s="15">
+        <f t="shared" si="12"/>
+        <v>1.1534995494142385E-4</v>
+      </c>
+      <c r="AI8" s="15">
+        <f>G8/SUM(G$2:G$11)*$AB8</f>
+        <v>6.8181818181818184E-5</v>
+      </c>
+      <c r="AJ8" s="15">
+        <f>SUM(F8:G8)/SUM(F$2:G$11)*AD8</f>
+        <v>1.1517696460707859E-4</v>
+      </c>
+      <c r="AK8" s="15">
+        <f t="shared" si="13"/>
+        <v>6000</v>
+      </c>
+      <c r="AL8" s="15">
+        <f t="shared" si="14"/>
+        <v>1.6118599745741265E-3</v>
+      </c>
+      <c r="AM8" s="15">
+        <f t="shared" si="15"/>
+        <v>3000</v>
+      </c>
+      <c r="AN8" s="15">
+        <f t="shared" si="16"/>
+        <v>8.1175161832933E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="str">
         <f>fundamental_data!A9</f>
         <v>Company H</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <f>fundamental_data!B9</f>
         <v>10008</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <f>fundamental_data!C9</f>
         <v>0</v>
       </c>
-      <c r="D9" s="4" t="str">
+      <c r="D9" s="3" t="str">
         <f>target_data!C9</f>
         <v>Absolute</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <f>target_data!D9</f>
         <v>0</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="10">
         <f>fundamental_data!D9</f>
         <v>75000</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <f>fundamental_data!E9</f>
         <v>35000</v>
       </c>
-      <c r="H9" s="4" t="str">
+      <c r="H9" s="3" t="str">
         <f>target_data!E9</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <f>target_data!F9</f>
         <v>1</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <f>target_data!G9</f>
         <v>1</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <f>target_data!H9</f>
         <v>1</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <f>target_data!J9</f>
         <v>2020</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <f>target_data!K9</f>
         <v>2034</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <f>target_data!I9</f>
         <v>0.7</v>
       </c>
-      <c r="O9" s="8">
+      <c r="O9" s="15">
+        <f>portfolio!E9</f>
+        <v>400000</v>
+      </c>
+      <c r="P9" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>2500000</v>
+      </c>
+      <c r="Q9" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P9" s="8">
+      <c r="R9" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q9" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S9" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R9" s="6">
+      <c r="T9" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S9" s="6">
+      <c r="U9" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T9" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V9" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U9" s="6">
+      <c r="W9" s="5">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="V9" s="6">
+      <c r="X9" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W9" s="6">
+      <c r="Y9" s="5">
         <f t="shared" si="4"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="X9" s="6">
+      <c r="Z9" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="AA9" s="9">
+        <f t="shared" si="9"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB9" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC9" s="9">
         <f t="shared" si="6"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="Z9" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA9" s="10">
-        <f t="shared" si="8"/>
         <v>0.31818181818181818</v>
       </c>
-      <c r="AB9" s="10">
-        <f t="shared" si="9"/>
-        <v>1.1356160000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="str">
+      <c r="AD9" s="9">
+        <f t="shared" si="11"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AE9" s="15">
+        <f>(O9*AA9)/SUM($O$2:$O$11)</f>
+        <v>6.2465753424657523E-2</v>
+      </c>
+      <c r="AF9" s="15">
+        <f>($O9*AB9)/SUM($O$2:$O$11)</f>
+        <v>6.2465753424657523E-2</v>
+      </c>
+      <c r="AG9" s="15">
+        <f>($O9*AD9)/SUM($O$2:$O$11)</f>
+        <v>6.2465753424657523E-2</v>
+      </c>
+      <c r="AH9" s="15">
+        <f t="shared" si="12"/>
+        <v>5.1366776809852804E-3</v>
+      </c>
+      <c r="AI9" s="15">
+        <f>G9/SUM(G$2:G$11)*$AB9</f>
+        <v>4.7727272727272722E-3</v>
+      </c>
+      <c r="AJ9" s="15">
+        <f>SUM(F9:G9)/SUM(F$2:G$11)*AD9</f>
+        <v>5.0149970005998797E-3</v>
+      </c>
+      <c r="AK9" s="15">
+        <f t="shared" si="13"/>
+        <v>12000</v>
+      </c>
+      <c r="AL9" s="15">
+        <f t="shared" si="14"/>
+        <v>1.9140837198067752E-3</v>
+      </c>
+      <c r="AM9" s="15">
+        <f t="shared" si="15"/>
+        <v>5600</v>
+      </c>
+      <c r="AN9" s="15">
+        <f t="shared" si="16"/>
+        <v>1.5152696875480828E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="str">
         <f>fundamental_data!A10</f>
         <v>Company I</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <f>fundamental_data!B10</f>
         <v>10009</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f>fundamental_data!C10</f>
         <v>0</v>
       </c>
-      <c r="D10" s="4" t="str">
+      <c r="D10" s="3" t="str">
         <f>target_data!C10</f>
         <v>Absolute</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <f>target_data!D10</f>
         <v>0</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="10">
         <f>fundamental_data!D10</f>
         <v>10000000</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <f>fundamental_data!E10</f>
         <v>4000000</v>
       </c>
-      <c r="H10" s="4" t="str">
+      <c r="H10" s="3" t="str">
         <f>target_data!E10</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <f>target_data!F10</f>
         <v>1</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <f>target_data!G10</f>
         <v>1</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <f>target_data!H10</f>
         <v>1</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <f>target_data!J10</f>
         <v>2020</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <f>target_data!K10</f>
         <v>2034</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <f>target_data!I10</f>
         <v>0.7</v>
       </c>
-      <c r="O10" s="8">
+      <c r="O10" s="15">
+        <f>portfolio!E10</f>
+        <v>500000</v>
+      </c>
+      <c r="P10" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>8000000</v>
+      </c>
+      <c r="Q10" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P10" s="8">
+      <c r="R10" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q10" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S10" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R10" s="6">
+      <c r="T10" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S10" s="6">
+      <c r="U10" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T10" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V10" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U10" s="6">
+      <c r="W10" s="5">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="V10" s="6">
+      <c r="X10" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W10" s="6">
+      <c r="Y10" s="5">
         <f t="shared" si="4"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="X10" s="6">
+      <c r="Z10" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y10" s="10">
+      <c r="AA10" s="9">
+        <f t="shared" si="9"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB10" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC10" s="9">
         <f t="shared" si="6"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="Z10" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA10" s="10">
-        <f t="shared" si="8"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="AB10" s="10">
-        <f t="shared" si="9"/>
-        <v>1.1356160000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="str">
+      <c r="AD10" s="9">
+        <f t="shared" si="11"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AE10" s="15">
+        <f>(O10*AA10)/SUM($O$2:$O$11)</f>
+        <v>7.8082191780821916E-2</v>
+      </c>
+      <c r="AF10" s="15">
+        <f>($O10*AB10)/SUM($O$2:$O$11)</f>
+        <v>7.8082191780821916E-2</v>
+      </c>
+      <c r="AG10" s="15">
+        <f>($O10*AD10)/SUM($O$2:$O$11)</f>
+        <v>7.8082191780821916E-2</v>
+      </c>
+      <c r="AH10" s="15">
+        <f t="shared" si="12"/>
+        <v>0.68489035746470406</v>
+      </c>
+      <c r="AI10" s="15">
+        <f>G10/SUM(G$2:G$11)*$AB10</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="AJ10" s="15">
+        <f>SUM(F10:G10)/SUM(F$2:G$11)*AD10</f>
+        <v>0.63827234553089385</v>
+      </c>
+      <c r="AK10" s="15">
+        <f t="shared" si="13"/>
+        <v>625000</v>
+      </c>
+      <c r="AL10" s="15">
+        <f t="shared" si="14"/>
+        <v>9.969186040660287E-2</v>
+      </c>
+      <c r="AM10" s="15">
+        <f t="shared" si="15"/>
+        <v>250000</v>
+      </c>
+      <c r="AN10" s="15">
+        <f t="shared" si="16"/>
+        <v>6.7645968194110825E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="str">
         <f>fundamental_data!A11</f>
         <v>Company J</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <f>fundamental_data!B11</f>
         <v>10010</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <f>fundamental_data!C11</f>
         <v>0</v>
       </c>
-      <c r="D11" s="4" t="str">
+      <c r="D11" s="3" t="str">
         <f>target_data!C11</f>
         <v>Absolute</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <f>target_data!D11</f>
         <v>0</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="10">
         <f>fundamental_data!D11</f>
         <v>4000</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <f>fundamental_data!E11</f>
         <v>2000</v>
       </c>
-      <c r="H11" s="4" t="str">
+      <c r="H11" s="3" t="str">
         <f>target_data!E11</f>
         <v>S1+S2+S3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <f>target_data!F11</f>
         <v>1</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <f>target_data!G11</f>
         <v>1</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <f>target_data!H11</f>
         <v>1</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <f>target_data!J11</f>
         <v>2020</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <f>target_data!K11</f>
         <v>2034</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <f>target_data!I11</f>
         <v>0.7</v>
       </c>
-      <c r="O11" s="8">
+      <c r="O11" s="15">
+        <f>portfolio!E11</f>
+        <v>150000</v>
+      </c>
+      <c r="P11" s="15">
+        <f>Table1[[#This Row],[company_revenue]]</f>
+        <v>250000</v>
+      </c>
+      <c r="Q11" s="7">
         <v>-0.31232900000000002</v>
       </c>
-      <c r="P11" s="8">
+      <c r="R11" s="7">
         <v>2.6972610000000001</v>
       </c>
-      <c r="Q11" s="6">
-        <f t="shared" ca="1" si="10"/>
+      <c r="S11" s="5">
+        <f t="shared" ca="1" si="7"/>
         <v>2021</v>
       </c>
-      <c r="R11" s="6">
+      <c r="T11" s="5">
         <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
-      <c r="S11" s="6">
+      <c r="U11" s="5">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="T11" s="6" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V11" s="5" t="str">
+        <f t="shared" ca="1" si="8"/>
         <v>mid</v>
       </c>
-      <c r="U11" s="6">
+      <c r="W11" s="5">
         <f t="shared" si="2"/>
         <v>0.7</v>
       </c>
-      <c r="V11" s="6">
+      <c r="X11" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
-      <c r="W11" s="6">
+      <c r="Y11" s="5">
         <f t="shared" si="4"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="X11" s="6">
+      <c r="Z11" s="5">
         <f t="shared" si="5"/>
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="Y11" s="10">
+      <c r="AA11" s="9">
+        <f t="shared" si="9"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AB11" s="9">
+        <f t="shared" si="10"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AC11" s="9">
         <f t="shared" si="6"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="Z11" s="10">
-        <f t="shared" si="7"/>
-        <v>1.1356160000000002</v>
-      </c>
-      <c r="AA11" s="10">
-        <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AB11" s="10">
-        <f t="shared" si="9"/>
-        <v>1.1356160000000002</v>
+      <c r="AD11" s="9">
+        <f t="shared" si="11"/>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AE11" s="15">
+        <f>(O11*AA11)/SUM($O$2:$O$11)</f>
+        <v>2.3424657534246572E-2</v>
+      </c>
+      <c r="AF11" s="15">
+        <f>($O11*AB11)/SUM($O$2:$O$11)</f>
+        <v>2.3424657534246572E-2</v>
+      </c>
+      <c r="AG11" s="15">
+        <f>($O11*AD11)/SUM($O$2:$O$11)</f>
+        <v>2.3424657534246572E-2</v>
+      </c>
+      <c r="AH11" s="15">
+        <f t="shared" si="12"/>
+        <v>2.7395614298588166E-4</v>
+      </c>
+      <c r="AI11" s="15">
+        <f>G11/SUM(G$2:G$11)*$AB11</f>
+        <v>2.7272727272727274E-4</v>
+      </c>
+      <c r="AJ11" s="15">
+        <f>SUM(F11:G11)/SUM(F$2:G$11)*AD11</f>
+        <v>2.7354529094181164E-4</v>
+      </c>
+      <c r="AK11" s="15">
+        <f t="shared" si="13"/>
+        <v>2400</v>
+      </c>
+      <c r="AL11" s="15">
+        <f t="shared" si="14"/>
+        <v>3.8281674396135505E-4</v>
+      </c>
+      <c r="AM11" s="15">
+        <f t="shared" si="15"/>
+        <v>1200</v>
+      </c>
+      <c r="AN11" s="15">
+        <f t="shared" si="16"/>
+        <v>3.2470064733173203E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AD12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE12">
+        <f>SUM(AE2:AE11)</f>
+        <v>1.5416095890410957</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" ref="AF12:AH12" si="17">SUM(AF2:AF11)</f>
+        <v>1.1482191780821915</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="17"/>
+        <v>1.5450342465753422</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="17"/>
+        <v>1.3104043256233102</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" ref="AI12" si="18">SUM(AI2:AI11)</f>
+        <v>1.190311004784689</v>
+      </c>
+      <c r="AJ12">
+        <f t="shared" ref="AJ12" si="19">SUM(AJ2:AJ11)</f>
+        <v>1.3360115976804638</v>
+      </c>
+      <c r="AL12">
+        <f>SUM(AL2:AL11)</f>
+        <v>1.6192760229201071</v>
+      </c>
+      <c r="AN12" s="15">
+        <f>SUM(AN2:AN11)</f>
+        <v>1.1514642114518441</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AA1:AA1048576">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="AC1:AC1048576">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
       <formula>0.4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0.67</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>